<commit_message>
Added the optional skip_nodes parameter to skip desired nodes
</commit_message>
<xml_diff>
--- a/NPCompleteness-TravelingSalesman/tsp_points.xlsx
+++ b/NPCompleteness-TravelingSalesman/tsp_points.xlsx
@@ -9,14 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16632" windowHeight="6480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16632" windowHeight="6480" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="simplified" sheetId="1" r:id="rId1"/>
     <sheet name="raw" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="tsp" localSheetId="1">raw!$A$1:$B$25</definedName>
+    <definedName name="tsp" localSheetId="2">Sheet1!$B$1:$C$11</definedName>
     <definedName name="tsp" localSheetId="0">simplified!$A$1:$B$21</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -39,6 +41,14 @@
     </textPr>
   </connection>
   <connection id="2" name="tsp1" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" firstRow="2" sourceFile="C:\Users\hghaed\Documents\GitHub\Course-Algorithm-Fall2016\NPCompleteness-TravelingSalesman\tsp.txt" space="1" consecutive="1">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="tsp11" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" firstRow="2" sourceFile="C:\Users\hghaed\Documents\GitHub\Course-Algorithm-Fall2016\NPCompleteness-TravelingSalesman\tsp.txt" space="1" consecutive="1">
       <textFields count="2">
         <textField/>
@@ -329,11 +339,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="203845888"/>
-        <c:axId val="203846280"/>
+        <c:axId val="139769416"/>
+        <c:axId val="139769800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="203845888"/>
+        <c:axId val="139769416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="20000"/>
@@ -391,12 +401,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203846280"/>
+        <c:crossAx val="139769800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="203846280"/>
+        <c:axId val="139769800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="8000"/>
@@ -454,7 +464,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203845888"/>
+        <c:crossAx val="139769416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -726,11 +736,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="203847456"/>
-        <c:axId val="203847848"/>
+        <c:axId val="155394952"/>
+        <c:axId val="155215240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="203847456"/>
+        <c:axId val="155394952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="20000"/>
@@ -788,12 +798,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203847848"/>
+        <c:crossAx val="155215240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="203847848"/>
+        <c:axId val="155215240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="8000"/>
@@ -851,7 +861,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203847456"/>
+        <c:crossAx val="155394952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2090,6 +2100,10 @@
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tsp" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tsp" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2355,8 +2369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="A1:B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2568,7 +2582,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="B25" sqref="A1:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2778,6 +2792,143 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>20833.333299999998</v>
+      </c>
+      <c r="C1">
+        <v>17100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>20900</v>
+      </c>
+      <c r="C2">
+        <v>17066.666700000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>21300</v>
+      </c>
+      <c r="C3">
+        <v>13016.6667</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>26433.333299999998</v>
+      </c>
+      <c r="C4">
+        <v>13433.3333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>26550</v>
+      </c>
+      <c r="C5">
+        <v>13850</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>26733.333299999998</v>
+      </c>
+      <c r="C6">
+        <v>11683.3333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>27026.111099999998</v>
+      </c>
+      <c r="C7">
+        <v>13051.9444</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>27096.111099999998</v>
+      </c>
+      <c r="C8">
+        <v>13415.8333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <v>27153.611099999998</v>
+      </c>
+      <c r="C9">
+        <v>13203.3333</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>27166.666700000002</v>
+      </c>
+      <c r="C10">
+        <v>9833.3333000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>25</v>
+      </c>
+      <c r="B11">
+        <v>27233.333299999998</v>
+      </c>
+      <c r="C11">
+        <v>10450</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>